<commit_message>
Warn about uncovered bill ranges
</commit_message>
<xml_diff>
--- a/example-bill.xlsx
+++ b/example-bill.xlsx
@@ -150,7 +150,7 @@
     <numFmt numFmtId="175" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -227,12 +227,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF404040"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -433,570 +427,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFD9D9D9"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF4472C4"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFC000"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFED7D31"/>
-      <rgbColor rgb="FF636363"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF70AD47"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF9E480E"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF264478"/>
-      <rgbColor rgb="FF404040"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472c4"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="a5a5a5"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffc000"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="5b9bd5"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="70ad47"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="264478"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="9e480e"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="636363"/>
-              </a:solidFill>
-              <a:ln w="19080">
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:numFmt formatCode="#,##0.00&quot; €&quot;" sourceLinked="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="404040"/>
-                      </a:solidFill>
-                      <a:latin typeface="Calibri"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator>; </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="404040"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="1"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Zusammenfassung!$B$5:$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Zusammenfassung!$D$5:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9360</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Diagramm 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="772200" y="4040640"/>
-        <a:ext cx="6886440" cy="5979240"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1007,7 +438,7 @@
   <dimension ref="B1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:D20"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1140,7 +571,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1152,7 +582,7 @@
   <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="1" sqref="B5:D20 M8"/>
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1483,7 +913,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="B5:D20"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>